<commit_message>
LaTeX: Intro suggestions Pierre
</commit_message>
<xml_diff>
--- a/TeX/P_related_coeffs.xlsx
+++ b/TeX/P_related_coeffs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>was in OMEN</t>
   </si>
@@ -32,13 +32,16 @@
     <t>Rate constant for P sorption (deep sea) ks</t>
   </si>
   <si>
+    <t>k0 in Palastanga is 0.019</t>
+  </si>
+  <si>
     <t>Rate constant for Fe-bound P release, km</t>
   </si>
   <si>
     <t>Until   0.24</t>
   </si>
   <si>
-    <t>k m is approximated as a background value (0.05 a −1 ) plus a rate dependent on the anaerobic degradation rate of POC, i.e. k m = 0.05 + k 0 (G 2 Cax /G C G Cax ) </t>
+    <t>k m is approximated as a background value (0.05 a −1 ) plus a rate dependent on the anaerobic degradation rate of POC, i.e. k m = 0.05 + k 0 (G 2 Cax /G C G Cax )</t>
   </si>
   <si>
     <t>Rate constant for authigenic Ca‐P precipitation, ka</t>
@@ -71,7 +74,7 @@
     <t>flux of M to the sediment</t>
   </si>
   <si>
-    <t>from Slomp et al. 1996 </t>
+    <t>from Slomp et al. 1996</t>
   </si>
   <si>
     <t>Fe-P in put (from Palastanga et al. 2011):</t>
@@ -108,6 +111,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,12 +133,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -142,6 +148,7 @@
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -295,7 +302,7 @@
   <dimension ref="B3:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -351,10 +358,13 @@
       <c r="D6" s="3" t="n">
         <v>3.65</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="n">
         <f aca="false">0.0000022*24*365</f>
@@ -365,15 +375,15 @@
         <v>0.05</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>10</v>
@@ -385,18 +395,18 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>1E-009</v>
@@ -411,7 +421,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>1E-009</v>
@@ -426,7 +436,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>1.99E-009</v>
@@ -441,7 +451,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>1.99E-009</v>
@@ -456,7 +466,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>3.7E-009</v>
@@ -471,12 +481,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">365*0.00000000002</f>
@@ -485,40 +495,40 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>